<commit_message>
Cambios en Excel (Primeras 30 Nomenclatura Binomial)
</commit_message>
<xml_diff>
--- a/Data/Ontology Data.xlsx
+++ b/Data/Ontology Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="344">
   <si>
     <t>Nombre</t>
   </si>
@@ -170,9 +170,6 @@
     <t>33-38 cm</t>
   </si>
   <si>
-    <t>Bat falcon</t>
-  </si>
-  <si>
     <t>23-30 cm</t>
   </si>
   <si>
@@ -960,13 +957,115 @@
   </si>
   <si>
     <t>Herpetotheres cachinnans</t>
+  </si>
+  <si>
+    <t>Melanerpes</t>
+  </si>
+  <si>
+    <t>Formicivorus</t>
+  </si>
+  <si>
+    <t>Melanerpes Formicivorus</t>
+  </si>
+  <si>
+    <t>Chloroceryle amazona</t>
+  </si>
+  <si>
+    <t>  Fulica americana</t>
+  </si>
+  <si>
+    <t>cinclus mexicanus</t>
+  </si>
+  <si>
+    <t>Charadriidae</t>
+  </si>
+  <si>
+    <t>  Pluvialis fulva</t>
+  </si>
+  <si>
+    <t>Haematopodidae</t>
+  </si>
+  <si>
+    <t> Haematopus palliatus</t>
+  </si>
+  <si>
+    <t>  Porphyrio martinicus</t>
+  </si>
+  <si>
+    <t> Eudocimus albus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pelecaniformes </t>
+  </si>
+  <si>
+    <t>  Anhinga anhinga</t>
+  </si>
+  <si>
+    <t>Laridae</t>
+  </si>
+  <si>
+    <t>Sterna paradisaea</t>
+  </si>
+  <si>
+    <t>Thraupidae</t>
+  </si>
+  <si>
+    <t>Coereba flaveola</t>
+  </si>
+  <si>
+    <t>Tyto alba</t>
+  </si>
+  <si>
+    <t>Tyto</t>
+  </si>
+  <si>
+    <t>Nystalus radiatus</t>
+  </si>
+  <si>
+    <t>Black falcon</t>
+  </si>
+  <si>
+    <t>Megaceryle alcyon</t>
+  </si>
+  <si>
+    <t>Cracidae</t>
+  </si>
+  <si>
+    <t>Chamaepetes unicolor</t>
+  </si>
+  <si>
+    <t>Coragyps atratus</t>
+  </si>
+  <si>
+    <t> Ciccaba nigrolineata</t>
+  </si>
+  <si>
+    <t>Dendrocygna autumnalis</t>
+  </si>
+  <si>
+    <t> Pittasoma michleri</t>
+  </si>
+  <si>
+    <t> Nycticorax nycticorax</t>
+  </si>
+  <si>
+    <t>Caryothraustes poliogaster</t>
+  </si>
+  <si>
+    <t> Ramphastos ambiguus</t>
+  </si>
+  <si>
+    <t> Trogon melanurus</t>
+  </si>
+  <si>
+    <t>Trogon rufus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -994,6 +1093,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="23">
@@ -1142,7 +1247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1193,6 +1298,7 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1517,7 +1623,7 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,158 +1663,171 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>270</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>271</v>
       </c>
       <c r="C2" s="37"/>
       <c r="D2" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" s="37" t="s">
         <v>272</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="F2" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="G2" s="37" t="s">
         <v>273</v>
       </c>
-      <c r="F2" s="38" t="s">
-        <v>268</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>274</v>
-      </c>
-      <c r="H2" t="e">
-        <f>LEFT(J2,FIND(" ",J2) -1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I2" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J2," ",REPT(" ",LEN(J2))),LEN(J2)))</f>
-        <v/>
+      <c r="H2" t="s">
+        <v>310</v>
+      </c>
+      <c r="I2" t="s">
+        <v>311</v>
+      </c>
+      <c r="J2" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>207</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>208</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>32</v>
       </c>
       <c r="F3" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="G3" s="29" t="s">
-        <v>210</v>
-      </c>
-      <c r="H3" t="e">
-        <f>LEFT(J3,FIND(" ",J3) -1)</f>
-        <v>#VALUE!</v>
+      <c r="H3" t="str">
+        <f t="shared" ref="H2:H13" si="0">LEFT(J3,FIND(" ",J3) -1)</f>
+        <v>Chloroceryle</v>
       </c>
       <c r="I3" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J3," ",REPT(" ",LEN(J3))),LEN(J3)))</f>
-        <v/>
+        <f t="shared" ref="I2:I13" si="1">TRIM(RIGHT(SUBSTITUTE(J3," ",REPT(" ",LEN(J3))),LEN(J3)))</f>
+        <v>amazona</v>
+      </c>
+      <c r="J3" s="29" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" t="e">
-        <f>LEFT(J4,FIND(" ",J4) -1)</f>
-        <v>#VALUE!</v>
+        <v>62</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>  Fulica</v>
       </c>
       <c r="I4" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J4," ",REPT(" ",LEN(J4))),LEN(J4)))</f>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>americana</v>
+      </c>
+      <c r="J4" s="42" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F5" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="H5" t="e">
-        <f>LEFT(J5,FIND(" ",J5) -1)</f>
-        <v>#VALUE!</v>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>cinclus</v>
       </c>
       <c r="I5" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J5," ",REPT(" ",LEN(J5))),LEN(J5)))</f>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>mexicanus</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>185</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>186</v>
       </c>
       <c r="C6" s="28"/>
       <c r="D6" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="E6" s="28" t="s">
-        <v>188</v>
-      </c>
       <c r="F6" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="H6" t="e">
-        <f>LEFT(J6,FIND(" ",J6) -1)</f>
-        <v>#VALUE!</v>
+        <v>316</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>  Pluvialis</v>
       </c>
       <c r="I6" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J6," ",REPT(" ",LEN(J6))),LEN(J6)))</f>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>fulva</v>
+      </c>
+      <c r="J6" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1732,189 +1851,207 @@
         <v>42</v>
       </c>
       <c r="H7" t="str">
-        <f>LEFT(J7,FIND(" ",J7) -1)</f>
+        <f t="shared" si="0"/>
         <v>Falco</v>
       </c>
       <c r="I7" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J7," ",REPT(" ",LEN(J7))),LEN(J7)))</f>
+        <f t="shared" si="1"/>
         <v>sparverius</v>
       </c>
       <c r="J7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" s="28" t="s">
         <v>189</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>190</v>
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="E8" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="E8" s="28" t="s">
-        <v>192</v>
-      </c>
       <c r="F8" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="H8" t="e">
-        <f>LEFT(J8,FIND(" ",J8) -1)</f>
-        <v>#VALUE!</v>
+        <v>318</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v> Haematopus</v>
       </c>
       <c r="I8" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J8," ",REPT(" ",LEN(J8))),LEN(J8)))</f>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>palliatus</v>
+      </c>
+      <c r="J8" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" t="e">
-        <f>LEFT(J9,FIND(" ",J9) -1)</f>
-        <v>#VALUE!</v>
+        <v>62</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>  Porphyrio</v>
       </c>
       <c r="I9" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J9," ",REPT(" ",LEN(J9))),LEN(J9)))</f>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>martinicus</v>
+      </c>
+      <c r="J9" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H10" t="e">
-        <f>LEFT(J10,FIND(" ",J10) -1)</f>
-        <v>#VALUE!</v>
+        <v>74</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v> Eudocimus</v>
       </c>
       <c r="I10" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J10," ",REPT(" ",LEN(J10))),LEN(J10)))</f>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>albus</v>
+      </c>
+      <c r="J10" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>112</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>113</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>111</v>
+        <v>322</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="H11" t="e">
-        <f>LEFT(J11,FIND(" ",J11) -1)</f>
-        <v>#VALUE!</v>
+        <v>113</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>  Anhinga</v>
       </c>
       <c r="I11" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J11," ",REPT(" ",LEN(J11))),LEN(J11)))</f>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>anhinga</v>
+      </c>
+      <c r="J11" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="E12" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="E12" s="28" t="s">
-        <v>195</v>
-      </c>
       <c r="F12" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="H12" t="e">
-        <f>LEFT(J12,FIND(" ",J12) -1)</f>
-        <v>#VALUE!</v>
+        <v>324</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>Sterna</v>
       </c>
       <c r="I12" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J12," ",REPT(" ",LEN(J12))),LEN(J12)))</f>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>paradisaea</v>
+      </c>
+      <c r="J12" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>234</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>235</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="H13" t="e">
-        <f>LEFT(J13,FIND(" ",J13) -1)</f>
-        <v>#VALUE!</v>
+        <v>326</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>Coereba</v>
       </c>
       <c r="I13" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J13," ",REPT(" ",LEN(J13))),LEN(J13)))</f>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>flaveola</v>
+      </c>
+      <c r="J13" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1938,10 +2075,10 @@
         <v>8</v>
       </c>
       <c r="H14" s="41" t="s">
+        <v>296</v>
+      </c>
+      <c r="I14" t="s">
         <v>297</v>
-      </c>
-      <c r="I14" t="s">
-        <v>298</v>
       </c>
       <c r="J14" t="str">
         <f>H14&amp;" " &amp; I14</f>
@@ -1950,27 +2087,33 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15" s="35" t="s">
         <v>253</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>254</v>
       </c>
       <c r="C15" s="35"/>
       <c r="D15" s="35" t="s">
+        <v>254</v>
+      </c>
+      <c r="E15" s="35" t="s">
         <v>255</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="F15" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="G15" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="F15" s="36" t="s">
-        <v>251</v>
-      </c>
-      <c r="G15" s="36" t="s">
-        <v>257</v>
+      <c r="H15" s="35" t="s">
+        <v>329</v>
       </c>
       <c r="I15" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J15," ",REPT(" ",LEN(J15))),LEN(J15)))</f>
-        <v/>
+        <f t="shared" ref="I15:I46" si="2">TRIM(RIGHT(SUBSTITUTE(J15," ",REPT(" ",LEN(J15))),LEN(J15)))</f>
+        <v>alba</v>
+      </c>
+      <c r="J15" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1994,56 +2137,59 @@
         <v>42</v>
       </c>
       <c r="H16" t="str">
-        <f>LEFT(J16,FIND(" ",J16) -1)</f>
+        <f t="shared" ref="H16:H47" si="3">LEFT(J16,FIND(" ",J16) -1)</f>
         <v>Micrastur</v>
       </c>
       <c r="I16" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J16," ",REPT(" ",LEN(J16))),LEN(J16)))</f>
+        <f t="shared" si="2"/>
         <v>ruficollis</v>
       </c>
       <c r="J16" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="G17" s="37" t="s">
         <v>280</v>
       </c>
-      <c r="E17" s="37" t="s">
-        <v>228</v>
-      </c>
-      <c r="F17" s="38" t="s">
-        <v>268</v>
-      </c>
-      <c r="G17" s="37" t="s">
-        <v>281</v>
-      </c>
-      <c r="H17" t="e">
-        <f>LEFT(J17,FIND(" ",J17) -1)</f>
-        <v>#VALUE!</v>
+      <c r="H17" t="str">
+        <f t="shared" si="3"/>
+        <v>Nystalus</v>
       </c>
       <c r="I17" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J17," ",REPT(" ",LEN(J17))),LEN(J17)))</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>radiatus</v>
+      </c>
+      <c r="J17" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>47</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>32</v>
@@ -2055,44 +2201,47 @@
         <v>42</v>
       </c>
       <c r="H18" t="str">
-        <f>LEFT(J18,FIND(" ",J18) -1)</f>
+        <f t="shared" si="3"/>
         <v>Falco</v>
       </c>
       <c r="I18" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J18," ",REPT(" ",LEN(J18))),LEN(J18)))</f>
+        <f t="shared" si="2"/>
         <v>rufigularis</v>
       </c>
       <c r="J18" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="B19" s="29" t="s">
         <v>211</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>212</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F19" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="G19" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="29" t="s">
-        <v>210</v>
-      </c>
-      <c r="H19" t="e">
-        <f>LEFT(J19,FIND(" ",J19) -1)</f>
-        <v>#VALUE!</v>
+      <c r="H19" t="str">
+        <f t="shared" si="3"/>
+        <v>Megaceryle</v>
       </c>
       <c r="I19" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J19," ",REPT(" ",LEN(J19))),LEN(J19)))</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>alcyon</v>
+      </c>
+      <c r="J19" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2116,339 +2265,369 @@
         <v>26</v>
       </c>
       <c r="H20" t="str">
-        <f>LEFT(J20,FIND(" ",J20) -1)</f>
+        <f t="shared" si="3"/>
         <v>Coccyzus</v>
       </c>
       <c r="I20" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J20," ",REPT(" ",LEN(J20))),LEN(J20)))</f>
+        <f t="shared" si="2"/>
         <v>erythropthalmus</v>
       </c>
       <c r="J20" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="B21" s="32" t="s">
         <v>225</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>226</v>
       </c>
       <c r="C21" s="32"/>
       <c r="D21" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="E21" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E21" s="32" t="s">
-        <v>228</v>
-      </c>
       <c r="F21" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>224</v>
-      </c>
-      <c r="H21" t="e">
-        <f>LEFT(J21,FIND(" ",J21) -1)</f>
-        <v>#VALUE!</v>
+        <v>333</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="3"/>
+        <v>Chamaepetes</v>
       </c>
       <c r="I21" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J21," ",REPT(" ",LEN(J21))),LEN(J21)))</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>unicolor</v>
+      </c>
+      <c r="J21" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>146</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>147</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E22" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="F22" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="G22" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="F22" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="H22" t="e">
-        <f>LEFT(J22,FIND(" ",J22) -1)</f>
-        <v>#VALUE!</v>
+      <c r="H22" t="str">
+        <f t="shared" si="3"/>
+        <v>Coragyps</v>
       </c>
       <c r="I22" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J22," ",REPT(" ",LEN(J22))),LEN(J22)))</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>atratus</v>
+      </c>
+      <c r="J22" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="B23" s="35" t="s">
         <v>264</v>
-      </c>
-      <c r="B23" s="35" t="s">
-        <v>265</v>
       </c>
       <c r="C23" s="35"/>
       <c r="D23" s="35" t="s">
         <v>28</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F23" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="G23" s="35" t="s">
         <v>251</v>
       </c>
-      <c r="G23" s="35" t="s">
-        <v>252</v>
-      </c>
-      <c r="H23" t="e">
-        <f>LEFT(J23,FIND(" ",J23) -1)</f>
-        <v>#VALUE!</v>
+      <c r="H23" t="str">
+        <f t="shared" si="3"/>
+        <v> Ciccaba</v>
       </c>
       <c r="I23" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J23," ",REPT(" ",LEN(J23))),LEN(J23)))</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>nigrolineata</v>
+      </c>
+      <c r="J23" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B24" s="24" t="s">
         <v>156</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>157</v>
       </c>
       <c r="C24" s="24"/>
       <c r="D24" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="E24" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>159</v>
-      </c>
       <c r="G24" s="25" t="s">
-        <v>289</v>
-      </c>
-      <c r="H24" t="e">
-        <f>LEFT(J24,FIND(" ",J24) -1)</f>
-        <v>#VALUE!</v>
+        <v>288</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="3"/>
+        <v>Dendrocygna</v>
       </c>
       <c r="I24" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J24," ",REPT(" ",LEN(J24))),LEN(J24)))</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>autumnalis</v>
+      </c>
+      <c r="J24" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="H25" t="e">
-        <f>LEFT(J25,FIND(" ",J25) -1)</f>
-        <v>#VALUE!</v>
+        <v>286</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="3"/>
+        <v> Pittasoma</v>
       </c>
       <c r="I25" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J25," ",REPT(" ",LEN(J25))),LEN(J25)))</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>michleri</v>
+      </c>
+      <c r="J25" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B26" s="40" t="s">
         <v>239</v>
-      </c>
-      <c r="B26" s="40" t="s">
-        <v>240</v>
       </c>
       <c r="C26" s="40"/>
       <c r="D26" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" s="40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F26" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G26" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="H26" t="e">
-        <f>LEFT(J26,FIND(" ",J26) -1)</f>
-        <v>#VALUE!</v>
+        <v>83</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="3"/>
+        <v> Nycticorax</v>
       </c>
       <c r="I26" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J26," ",REPT(" ",LEN(J26))),LEN(J26)))</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>nycticorax</v>
+      </c>
+      <c r="J26" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F27" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="G27" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="G27" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="H27" t="e">
-        <f>LEFT(J27,FIND(" ",J27) -1)</f>
-        <v>#VALUE!</v>
+      <c r="H27" t="str">
+        <f t="shared" si="3"/>
+        <v>Caryothraustes</v>
       </c>
       <c r="I27" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J27," ",REPT(" ",LEN(J27))),LEN(J27)))</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>poliogaster</v>
+      </c>
+      <c r="J27" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="B28" s="37" t="s">
         <v>266</v>
-      </c>
-      <c r="B28" s="37" t="s">
-        <v>267</v>
       </c>
       <c r="C28" s="37"/>
       <c r="D28" s="37" t="s">
         <v>28</v>
       </c>
       <c r="E28" s="37" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F28" s="37" t="s">
+        <v>267</v>
+      </c>
+      <c r="G28" s="37" t="s">
         <v>268</v>
       </c>
-      <c r="G28" s="37" t="s">
-        <v>269</v>
-      </c>
-      <c r="H28" t="e">
-        <f>LEFT(J28,FIND(" ",J28) -1)</f>
-        <v>#VALUE!</v>
+      <c r="H28" t="str">
+        <f t="shared" si="3"/>
+        <v> Ramphastos</v>
       </c>
       <c r="I28" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J28," ",REPT(" ",LEN(J28))),LEN(J28)))</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>ambiguus</v>
+      </c>
+      <c r="J28" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C29" s="33"/>
       <c r="D29" s="33" t="s">
         <v>28</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F29" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="G29" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="G29" s="33" t="s">
-        <v>243</v>
-      </c>
-      <c r="H29" t="e">
-        <f>LEFT(J29,FIND(" ",J29) -1)</f>
-        <v>#VALUE!</v>
+      <c r="H29" t="str">
+        <f t="shared" si="3"/>
+        <v> Trogon</v>
       </c>
       <c r="I29" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J29," ",REPT(" ",LEN(J29))),LEN(J29)))</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>melanurus</v>
+      </c>
+      <c r="J29" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="B30" s="33" t="s">
         <v>246</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>247</v>
       </c>
       <c r="C30" s="33"/>
       <c r="D30" s="33" t="s">
         <v>28</v>
       </c>
       <c r="E30" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="G30" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="G30" s="33" t="s">
-        <v>243</v>
-      </c>
-      <c r="H30" t="e">
-        <f>LEFT(J30,FIND(" ",J30) -1)</f>
-        <v>#VALUE!</v>
+      <c r="H30" t="str">
+        <f t="shared" si="3"/>
+        <v>Trogon</v>
       </c>
       <c r="I30" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J30," ",REPT(" ",LEN(J30))),LEN(J30)))</f>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>rufus</v>
+      </c>
+      <c r="J30" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="14" t="s">
         <v>124</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>125</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H31" t="e">
-        <f>LEFT(J31,FIND(" ",J31) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I31" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J31," ",REPT(" ",LEN(J31))),LEN(J31)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>37</v>
@@ -2461,191 +2640,191 @@
         <v>32</v>
       </c>
       <c r="F32" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="G32" s="17" t="s">
-        <v>100</v>
-      </c>
       <c r="H32" t="e">
-        <f>LEFT(J32,FIND(" ",J32) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I32" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J32," ",REPT(" ",LEN(J32))),LEN(J32)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="B33" s="29" t="s">
         <v>214</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>215</v>
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="G33" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="G33" s="29" t="s">
-        <v>210</v>
-      </c>
       <c r="H33" t="e">
-        <f>LEFT(J33,FIND(" ",J33) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I33" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J33," ",REPT(" ",LEN(J33))),LEN(J33)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="B34" s="29" t="s">
         <v>216</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>217</v>
       </c>
       <c r="C34" s="29"/>
       <c r="D34" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F34" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="G34" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="G34" s="29" t="s">
-        <v>210</v>
-      </c>
       <c r="H34" t="e">
-        <f>LEFT(J34,FIND(" ",J34) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I34" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J34," ",REPT(" ",LEN(J34))),LEN(J34)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H35" t="e">
-        <f>LEFT(J35,FIND(" ",J35) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I35" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J35," ",REPT(" ",LEN(J35))),LEN(J35)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="35" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B36" s="35" t="s">
         <v>44</v>
       </c>
       <c r="C36" s="35"/>
       <c r="D36" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="E36" s="35" t="s">
         <v>262</v>
       </c>
-      <c r="E36" s="35" t="s">
-        <v>263</v>
-      </c>
       <c r="F36" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="G36" s="35" t="s">
         <v>251</v>
       </c>
-      <c r="G36" s="35" t="s">
-        <v>252</v>
-      </c>
       <c r="H36" t="e">
-        <f>LEFT(J36,FIND(" ",J36) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I36" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J36," ",REPT(" ",LEN(J36))),LEN(J36)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="16" t="s">
         <v>102</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="C37" s="16"/>
       <c r="D37" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F37" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G37" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="G37" s="17" t="s">
-        <v>100</v>
-      </c>
       <c r="H37" t="e">
-        <f>LEFT(J37,FIND(" ",J37) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I37" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J37," ",REPT(" ",LEN(J37))),LEN(J37)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H38" t="e">
-        <f>LEFT(J38,FIND(" ",J38) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I38" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J38," ",REPT(" ",LEN(J38))),LEN(J38)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -2670,246 +2849,246 @@
         <v>8</v>
       </c>
       <c r="H39" t="str">
-        <f>LEFT(J39,FIND(" ",J39) -1)</f>
+        <f t="shared" si="3"/>
         <v>Columbina</v>
       </c>
       <c r="I39" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J39," ",REPT(" ",LEN(J39))),LEN(J39)))</f>
+        <f t="shared" si="2"/>
         <v>passerina</v>
       </c>
       <c r="J39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="27" t="s">
         <v>169</v>
-      </c>
-      <c r="B40" s="27" t="s">
-        <v>170</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E40" s="27" t="s">
         <v>19</v>
       </c>
       <c r="F40" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="G40" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="G40" s="27" t="s">
-        <v>173</v>
-      </c>
       <c r="H40" t="e">
-        <f>LEFT(J40,FIND(" ",J40) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I40" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J40," ",REPT(" ",LEN(J40))),LEN(J40)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" s="27" t="s">
         <v>174</v>
-      </c>
-      <c r="B41" s="27" t="s">
-        <v>175</v>
       </c>
       <c r="C41" s="27"/>
       <c r="D41" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F41" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="G41" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="G41" s="27" t="s">
-        <v>173</v>
-      </c>
       <c r="H41" t="e">
-        <f>LEFT(J41,FIND(" ",J41) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I41" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J41," ",REPT(" ",LEN(J41))),LEN(J41)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="B42" s="36" t="s">
         <v>258</v>
-      </c>
-      <c r="B42" s="36" t="s">
-        <v>259</v>
       </c>
       <c r="C42" s="35"/>
       <c r="D42" s="36" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E42" s="35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F42" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="G42" s="35" t="s">
         <v>251</v>
       </c>
-      <c r="G42" s="35" t="s">
-        <v>252</v>
-      </c>
       <c r="H42" t="e">
-        <f>LEFT(J42,FIND(" ",J42) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I42" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J42," ",REPT(" ",LEN(J42))),LEN(J42)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B43" s="32" t="s">
         <v>44</v>
       </c>
       <c r="C43" s="32"/>
       <c r="D43" s="32" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E43" s="32" t="s">
         <v>32</v>
       </c>
       <c r="F43" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="G43" s="32" t="s">
         <v>223</v>
       </c>
-      <c r="G43" s="32" t="s">
-        <v>224</v>
-      </c>
       <c r="H43" t="e">
-        <f>LEFT(J43,FIND(" ",J43) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I43" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J43," ",REPT(" ",LEN(J43))),LEN(J43)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B44" s="28" t="s">
         <v>30</v>
       </c>
       <c r="C44" s="28"/>
       <c r="D44" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E44" s="28" t="s">
         <v>32</v>
       </c>
       <c r="F44" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="G44" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="G44" s="28" t="s">
-        <v>184</v>
-      </c>
       <c r="H44" t="e">
-        <f>LEFT(J44,FIND(" ",J44) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I44" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J44," ",REPT(" ",LEN(J44))),LEN(J44)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B45" s="24" t="s">
         <v>40</v>
       </c>
       <c r="C45" s="24"/>
       <c r="D45" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F45" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G45" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H45" t="e">
-        <f>LEFT(J45,FIND(" ",J45) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I45" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J45," ",REPT(" ",LEN(J45))),LEN(J45)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B46" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C46" s="33"/>
       <c r="D46" s="33" t="s">
         <v>28</v>
       </c>
       <c r="E46" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F46" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="G46" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="G46" s="33" t="s">
-        <v>243</v>
-      </c>
       <c r="H46" t="e">
-        <f>LEFT(J46,FIND(" ",J46) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I46" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J46," ",REPT(" ",LEN(J46))),LEN(J46)))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="37" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C47" s="37"/>
       <c r="D47" s="37" t="s">
         <v>28</v>
       </c>
       <c r="E47" s="37" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F47" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G47" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H47" t="e">
-        <f>LEFT(J47,FIND(" ",J47) -1)</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I47" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J47," ",REPT(" ",LEN(J47))),LEN(J47)))</f>
+        <f t="shared" ref="I47:I78" si="4">TRIM(RIGHT(SUBSTITUTE(J47," ",REPT(" ",LEN(J47))),LEN(J47)))</f>
         <v/>
       </c>
     </row>
@@ -2934,43 +3113,43 @@
         <v>26</v>
       </c>
       <c r="H48" t="str">
-        <f>LEFT(J48,FIND(" ",J48) -1)</f>
+        <f t="shared" ref="H48:H64" si="5">LEFT(J48,FIND(" ",J48) -1)</f>
         <v>Crotophaga</v>
       </c>
       <c r="I48" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J48," ",REPT(" ",LEN(J48))),LEN(J48)))</f>
+        <f t="shared" si="4"/>
         <v>major</v>
       </c>
       <c r="J48" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B49" s="33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C49" s="33"/>
       <c r="D49" s="33" t="s">
         <v>28</v>
       </c>
       <c r="E49" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F49" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="G49" s="34" t="s">
         <v>242</v>
       </c>
-      <c r="G49" s="34" t="s">
-        <v>243</v>
-      </c>
       <c r="H49" t="e">
-        <f>LEFT(J49,FIND(" ",J49) -1)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="I49" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J49," ",REPT(" ",LEN(J49))),LEN(J49)))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2995,117 +3174,117 @@
         <v>26</v>
       </c>
       <c r="H50" t="str">
-        <f>LEFT(J50,FIND(" ",J50) -1)</f>
+        <f t="shared" si="5"/>
         <v>Crotophaga</v>
       </c>
       <c r="I50" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J50," ",REPT(" ",LEN(J50))),LEN(J50)))</f>
+        <f t="shared" si="4"/>
         <v>sulcirostris</v>
       </c>
       <c r="J50" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B51" s="20" t="s">
         <v>137</v>
-      </c>
-      <c r="B51" s="20" t="s">
-        <v>138</v>
       </c>
       <c r="C51" s="20"/>
       <c r="D51" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="E51" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="E51" s="21" t="s">
+      <c r="F51" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="F51" s="20" t="s">
+      <c r="G51" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="G51" s="20" t="s">
-        <v>142</v>
-      </c>
       <c r="H51" t="e">
-        <f>LEFT(J51,FIND(" ",J51) -1)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="I51" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J51," ",REPT(" ",LEN(J51))),LEN(J51)))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F52" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G52" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="G52" s="4" t="s">
-        <v>202</v>
-      </c>
       <c r="H52" t="e">
-        <f>LEFT(J52,FIND(" ",J52) -1)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="I52" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J52," ",REPT(" ",LEN(J52))),LEN(J52)))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B53" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C53" s="33"/>
       <c r="D53" s="34" t="s">
         <v>28</v>
       </c>
       <c r="E53" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F53" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="G53" s="34" t="s">
         <v>242</v>
       </c>
-      <c r="G53" s="34" t="s">
-        <v>243</v>
-      </c>
       <c r="H53" t="e">
-        <f>LEFT(J53,FIND(" ",J53) -1)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="I53" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J53," ",REPT(" ",LEN(J53))),LEN(J53)))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="12" t="s">
         <v>54</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>55</v>
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="12" t="s">
         <v>28</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F54" s="12" t="s">
         <v>41</v>
@@ -3114,130 +3293,130 @@
         <v>42</v>
       </c>
       <c r="H54" t="str">
-        <f>LEFT(J54,FIND(" ",J54) -1)</f>
+        <f t="shared" si="5"/>
         <v>Herpetotheres</v>
       </c>
       <c r="I54" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J54," ",REPT(" ",LEN(J54))),LEN(J54)))</f>
+        <f t="shared" si="4"/>
         <v>cachinnans</v>
       </c>
       <c r="J54" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H55" t="e">
-        <f>LEFT(J55,FIND(" ",J55) -1)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="I55" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J55," ",REPT(" ",LEN(J55))),LEN(J55)))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="B56" s="27" t="s">
         <v>176</v>
-      </c>
-      <c r="B56" s="27" t="s">
-        <v>177</v>
       </c>
       <c r="C56" s="27"/>
       <c r="D56" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E56" s="27" t="s">
         <v>12</v>
       </c>
       <c r="F56" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="G56" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="G56" s="27" t="s">
-        <v>173</v>
-      </c>
       <c r="H56" t="e">
-        <f>LEFT(J56,FIND(" ",J56) -1)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="I56" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J56," ",REPT(" ",LEN(J56))),LEN(J56)))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B57" s="24" t="s">
         <v>162</v>
-      </c>
-      <c r="B57" s="24" t="s">
-        <v>163</v>
       </c>
       <c r="C57" s="24"/>
       <c r="D57" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E57" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F57" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G57" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H57" t="e">
-        <f>LEFT(J57,FIND(" ",J57) -1)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="I57" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J57," ",REPT(" ",LEN(J57))),LEN(J57)))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="C58" s="6"/>
       <c r="D58" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H58" t="e">
-        <f>LEFT(J58,FIND(" ",J58) -1)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="I58" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J58," ",REPT(" ",LEN(J58))),LEN(J58)))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -3262,159 +3441,159 @@
         <v>26</v>
       </c>
       <c r="H59" t="str">
-        <f>LEFT(J59,FIND(" ",J59) -1)</f>
+        <f t="shared" si="5"/>
         <v>Coccycua</v>
       </c>
       <c r="I59" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J59," ",REPT(" ",LEN(J59))),LEN(J59)))</f>
+        <f t="shared" si="4"/>
         <v>minuta</v>
       </c>
       <c r="J59" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B60" s="18" t="s">
         <v>134</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>135</v>
       </c>
       <c r="C60" s="18"/>
       <c r="D60" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F60" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G60" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="G60" s="19" t="s">
-        <v>133</v>
-      </c>
       <c r="H60" t="e">
-        <f>LEFT(J60,FIND(" ",J60) -1)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="I60" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J60," ",REPT(" ",LEN(J60))),LEN(J60)))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="F61" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G61" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G61" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="H61" t="e">
-        <f>LEFT(J61,FIND(" ",J61) -1)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="I61" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J61," ",REPT(" ",LEN(J61))),LEN(J61)))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B62" s="14" t="s">
         <v>115</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>116</v>
       </c>
       <c r="C62" s="14"/>
       <c r="D62" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="G62" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E62" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="F62" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="G62" s="15" t="s">
-        <v>118</v>
-      </c>
       <c r="H62" t="e">
-        <f>LEFT(J62,FIND(" ",J62) -1)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="I62" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J62," ",REPT(" ",LEN(J62))),LEN(J62)))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F63" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G63" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="G63" s="4" t="s">
-        <v>202</v>
-      </c>
       <c r="H63" t="e">
-        <f>LEFT(J63,FIND(" ",J63) -1)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="I63" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J63," ",REPT(" ",LEN(J63))),LEN(J63)))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B64" s="16" t="s">
         <v>105</v>
-      </c>
-      <c r="B64" s="16" t="s">
-        <v>106</v>
       </c>
       <c r="C64" s="16"/>
       <c r="D64" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F64" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G64" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="G64" s="17" t="s">
-        <v>100</v>
-      </c>
       <c r="H64" t="e">
-        <f>LEFT(J64,FIND(" ",J64) -1)</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="I64" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J64," ",REPT(" ",LEN(J64))),LEN(J64)))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -3439,10 +3618,10 @@
         <v>8</v>
       </c>
       <c r="H65" s="41" t="s">
+        <v>294</v>
+      </c>
+      <c r="I65" s="41" t="s">
         <v>295</v>
-      </c>
-      <c r="I65" s="41" t="s">
-        <v>296</v>
       </c>
       <c r="J65" s="41" t="str">
         <f>H65&amp;" " &amp; I65</f>
@@ -3451,162 +3630,162 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="B66" s="24" t="s">
         <v>164</v>
-      </c>
-      <c r="B66" s="24" t="s">
-        <v>165</v>
       </c>
       <c r="C66" s="24"/>
       <c r="D66" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E66" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F66" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G66" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H66" t="e">
-        <f>LEFT(J66,FIND(" ",J66) -1)</f>
+        <f t="shared" ref="H66:H79" si="6">LEFT(J66,FIND(" ",J66) -1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="I66" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J66," ",REPT(" ",LEN(J66))),LEN(J66)))</f>
+        <f t="shared" ref="I66:I79" si="7">TRIM(RIGHT(SUBSTITUTE(J66," ",REPT(" ",LEN(J66))),LEN(J66)))</f>
         <v/>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B67" s="14" t="s">
         <v>120</v>
-      </c>
-      <c r="B67" s="14" t="s">
-        <v>121</v>
       </c>
       <c r="C67" s="14"/>
       <c r="D67" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E67" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H67" t="e">
-        <f>LEFT(J67,FIND(" ",J67) -1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="I67" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J67," ",REPT(" ",LEN(J67))),LEN(J67)))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C68" s="24"/>
       <c r="D68" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E68" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F68" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G68" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H68" t="e">
-        <f>LEFT(J68,FIND(" ",J68) -1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="I68" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J68," ",REPT(" ",LEN(J68))),LEN(J68)))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="B69" s="27" t="s">
         <v>178</v>
-      </c>
-      <c r="B69" s="27" t="s">
-        <v>179</v>
       </c>
       <c r="C69" s="27"/>
       <c r="D69" s="27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E69" s="27" t="s">
         <v>32</v>
       </c>
       <c r="F69" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="G69" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="G69" s="27" t="s">
-        <v>173</v>
-      </c>
       <c r="H69" t="e">
-        <f>LEFT(J69,FIND(" ",J69) -1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="I69" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J69," ",REPT(" ",LEN(J69))),LEN(J69)))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B70" s="16" t="s">
         <v>107</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>108</v>
       </c>
       <c r="C70" s="16"/>
       <c r="D70" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F70" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G70" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="G70" s="17" t="s">
-        <v>100</v>
-      </c>
       <c r="H70" t="e">
-        <f>LEFT(J70,FIND(" ",J70) -1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="I70" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J70," ",REPT(" ",LEN(J70))),LEN(J70)))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B71" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="C71" s="12"/>
       <c r="D71" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E71" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="E71" s="12" t="s">
-        <v>53</v>
       </c>
       <c r="F71" s="12" t="s">
         <v>41</v>
@@ -3615,23 +3794,23 @@
         <v>42</v>
       </c>
       <c r="H71" t="str">
-        <f>LEFT(J71,FIND(" ",J71) -1)</f>
+        <f t="shared" si="6"/>
         <v>Falco</v>
       </c>
       <c r="I71" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J71," ",REPT(" ",LEN(J71))),LEN(J71)))</f>
+        <f t="shared" si="7"/>
         <v>peregrinus</v>
       </c>
       <c r="J71" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
@@ -3641,17 +3820,17 @@
         <v>12</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H72" t="e">
-        <f>LEFT(J72,FIND(" ",J72) -1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="I72" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J72," ",REPT(" ",LEN(J72))),LEN(J72)))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3676,188 +3855,188 @@
         <v>8</v>
       </c>
       <c r="H73" t="str">
-        <f>LEFT(J73,FIND(" ",J73) -1)</f>
+        <f t="shared" si="6"/>
         <v>Columbina</v>
       </c>
       <c r="I73" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J73," ",REPT(" ",LEN(J73))),LEN(J73)))</f>
+        <f t="shared" si="7"/>
         <v>minuta</v>
       </c>
       <c r="J73" s="41" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="B74" s="28" t="s">
         <v>196</v>
-      </c>
-      <c r="B74" s="28" t="s">
-        <v>197</v>
       </c>
       <c r="C74" s="28"/>
       <c r="D74" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E74" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F74" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="G74" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="G74" s="28" t="s">
-        <v>184</v>
-      </c>
       <c r="H74" t="e">
-        <f>LEFT(J74,FIND(" ",J74) -1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="I74" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J74," ",REPT(" ",LEN(J74))),LEN(J74)))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B75" s="14" t="s">
         <v>128</v>
-      </c>
-      <c r="B75" s="14" t="s">
-        <v>129</v>
       </c>
       <c r="C75" s="14"/>
       <c r="D75" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E75" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E75" s="14" t="s">
-        <v>131</v>
-      </c>
       <c r="F75" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H75" t="e">
-        <f>LEFT(J75,FIND(" ",J75) -1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="I75" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J75," ",REPT(" ",LEN(J75))),LEN(J75)))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B76" s="16" t="s">
         <v>109</v>
-      </c>
-      <c r="B76" s="16" t="s">
-        <v>110</v>
       </c>
       <c r="C76" s="16"/>
       <c r="D76" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E76" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F76" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G76" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="G76" s="17" t="s">
-        <v>100</v>
-      </c>
       <c r="H76" t="e">
-        <f>LEFT(J76,FIND(" ",J76) -1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="I76" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J76," ",REPT(" ",LEN(J76))),LEN(J76)))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="B77" s="39" t="s">
         <v>282</v>
-      </c>
-      <c r="B77" s="39" t="s">
-        <v>283</v>
       </c>
       <c r="C77" s="39"/>
       <c r="D77" s="39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E77" s="39" t="s">
+        <v>283</v>
+      </c>
+      <c r="F77" s="39" t="s">
         <v>284</v>
       </c>
-      <c r="F77" s="39" t="s">
+      <c r="G77" s="39" t="s">
         <v>285</v>
       </c>
-      <c r="G77" s="39" t="s">
-        <v>286</v>
-      </c>
       <c r="H77" t="e">
-        <f>LEFT(J77,FIND(" ",J77) -1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="I77" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J77," ",REPT(" ",LEN(J77))),LEN(J77)))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B78" s="37" t="s">
         <v>21</v>
       </c>
       <c r="C78" s="37"/>
       <c r="D78" s="37" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E78" s="37" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F78" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G78" s="37" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H78" t="e">
-        <f>LEFT(J78,FIND(" ",J78) -1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="I78" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J78," ",REPT(" ",LEN(J78))),LEN(J78)))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B79" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="C79" s="4"/>
       <c r="D79" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H79" t="e">
-        <f>LEFT(J79,FIND(" ",J79) -1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="I79" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J79," ",REPT(" ",LEN(J79))),LEN(J79)))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3882,10 +4061,10 @@
         <v>8</v>
       </c>
       <c r="H80" s="41" t="s">
+        <v>292</v>
+      </c>
+      <c r="I80" s="41" t="s">
         <v>293</v>
-      </c>
-      <c r="I80" s="41" t="s">
-        <v>294</v>
       </c>
       <c r="J80" s="41" t="str">
         <f>H80&amp;" " &amp; I80</f>
@@ -3894,146 +4073,146 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="B81" s="29" t="s">
         <v>218</v>
-      </c>
-      <c r="B81" s="29" t="s">
-        <v>219</v>
       </c>
       <c r="C81" s="29"/>
       <c r="D81" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E81" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F81" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="G81" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="G81" s="29" t="s">
-        <v>210</v>
-      </c>
       <c r="H81" t="e">
-        <f>LEFT(J81,FIND(" ",J81) -1)</f>
+        <f t="shared" ref="H81:H91" si="8">LEFT(J81,FIND(" ",J81) -1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="I81" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J81," ",REPT(" ",LEN(J81))),LEN(J81)))</f>
+        <f t="shared" ref="I81:I91" si="9">TRIM(RIGHT(SUBSTITUTE(J81," ",REPT(" ",LEN(J81))),LEN(J81)))</f>
         <v/>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B82" s="20" t="s">
         <v>153</v>
-      </c>
-      <c r="B82" s="20" t="s">
-        <v>154</v>
       </c>
       <c r="C82" s="20"/>
       <c r="D82" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E82" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F82" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="G82" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="G82" s="20" t="s">
-        <v>142</v>
-      </c>
       <c r="H82" t="e">
-        <f>LEFT(J82,FIND(" ",J82) -1)</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="I82" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J82," ",REPT(" ",LEN(J82))),LEN(J82)))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H83" t="e">
-        <f>LEFT(J83,FIND(" ",J83) -1)</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="I83" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J83," ",REPT(" ",LEN(J83))),LEN(J83)))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H84" t="e">
-        <f>LEFT(J84,FIND(" ",J84) -1)</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="I84" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J84," ",REPT(" ",LEN(J84))),LEN(J84)))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="B85" s="35" t="s">
         <v>249</v>
-      </c>
-      <c r="B85" s="35" t="s">
-        <v>250</v>
       </c>
       <c r="C85" s="35"/>
       <c r="D85" s="35" t="s">
         <v>28</v>
       </c>
       <c r="E85" s="35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F85" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="G85" s="36" t="s">
         <v>251</v>
       </c>
-      <c r="G85" s="36" t="s">
-        <v>252</v>
-      </c>
       <c r="H85" t="e">
-        <f>LEFT(J85,FIND(" ",J85) -1)</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="I85" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J85," ",REPT(" ",LEN(J85))),LEN(J85)))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -4058,159 +4237,159 @@
         <v>26</v>
       </c>
       <c r="H86" t="str">
-        <f>LEFT(J86,FIND(" ",J86) -1)</f>
+        <f t="shared" si="8"/>
         <v>Piaya</v>
       </c>
       <c r="I86" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J86," ",REPT(" ",LEN(J86))),LEN(J86)))</f>
+        <f t="shared" si="9"/>
         <v>cayana</v>
       </c>
       <c r="J86" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="B87" s="31" t="s">
         <v>220</v>
-      </c>
-      <c r="B87" s="31" t="s">
-        <v>221</v>
       </c>
       <c r="C87" s="31"/>
       <c r="D87" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E87" s="31" t="s">
         <v>32</v>
       </c>
       <c r="F87" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="G87" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="G87" s="31" t="s">
-        <v>210</v>
-      </c>
       <c r="H87" t="e">
-        <f>LEFT(J87,FIND(" ",J87) -1)</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="I87" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J87," ",REPT(" ",LEN(J87))),LEN(J87)))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C88" s="6"/>
       <c r="D88" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G88" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E88" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F88" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G88" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="H88" t="e">
-        <f>LEFT(J88,FIND(" ",J88) -1)</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="I88" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J88," ",REPT(" ",LEN(J88))),LEN(J88)))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B89" s="20" t="s">
         <v>151</v>
-      </c>
-      <c r="B89" s="20" t="s">
-        <v>152</v>
       </c>
       <c r="C89" s="20"/>
       <c r="D89" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="E89" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="E89" s="22" t="s">
+      <c r="F89" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F89" s="23" t="s">
+      <c r="G89" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="G89" s="20" t="s">
-        <v>142</v>
-      </c>
       <c r="H89" t="e">
-        <f>LEFT(J89,FIND(" ",J89) -1)</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="I89" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J89," ",REPT(" ",LEN(J89))),LEN(J89)))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B90" s="20" t="s">
         <v>143</v>
-      </c>
-      <c r="B90" s="20" t="s">
-        <v>144</v>
       </c>
       <c r="C90" s="20"/>
       <c r="D90" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E90" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="F90" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="F90" s="20" t="s">
+      <c r="G90" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="G90" s="20" t="s">
-        <v>142</v>
-      </c>
       <c r="H90" t="e">
-        <f>LEFT(J90,FIND(" ",J90) -1)</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="I90" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J90," ",REPT(" ",LEN(J90))),LEN(J90)))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B91" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="C91" s="4"/>
       <c r="D91" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F91" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G91" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="G91" s="4" t="s">
-        <v>202</v>
-      </c>
       <c r="H91" t="e">
-        <f>LEFT(J91,FIND(" ",J91) -1)</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="I91" t="str">
-        <f>TRIM(RIGHT(SUBSTITUTE(J91," ",REPT(" ",LEN(J91))),LEN(J91)))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>

</xml_diff>